<commit_message>
Added 2nd sheet with tables for the report
</commit_message>
<xml_diff>
--- a/Results_Comparison.xlsx
+++ b/Results_Comparison.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\MDS\labs\block4\data_553\project\data553_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdlee\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACD9ECF-B787-491B-A433-0FEADC099459}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309C2D80-850E-40CC-BBDF-63FDADBF00EA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5B1D236F-2377-4A5F-BEB3-C9DD1F3CC62D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Figures" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$H$6:$J$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="18">
   <si>
     <t>Precision</t>
   </si>
@@ -71,12 +75,30 @@
   <si>
     <t>BOW + lemmatization</t>
   </si>
+  <si>
+    <t>BOW +      Rating + Lemmatization</t>
+  </si>
+  <si>
+    <t>BOW +   Bigrams - Stopwords + Lemmatization</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Review Count</t>
+  </si>
+  <si>
+    <t>% of Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +106,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -101,15 +144,280 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -205,7 +513,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Figures!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -285,7 +593,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$3:$B$16</c:f>
+              <c:f>Figures!$A$3:$B$16</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
@@ -351,7 +659,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$16</c:f>
+              <c:f>Figures!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -405,7 +713,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Figures!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -485,7 +793,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$3:$B$16</c:f>
+              <c:f>Figures!$A$3:$B$16</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
@@ -551,7 +859,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$16</c:f>
+              <c:f>Figures!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -608,7 +916,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="59"/>
         <c:overlap val="-27"/>
         <c:axId val="21650815"/>
         <c:axId val="96254095"/>
@@ -839,7 +1147,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>BOW + bigrams - stopwords + lemmatization</a:t>
+              <a:t>BOW + Bigrams - Stopwords + Lemmatization</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -885,7 +1193,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Figures!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,6 +1244,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -965,7 +1274,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$3:$B$16</c:f>
+              <c:f>Figures!$A$3:$B$16</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
@@ -1031,7 +1340,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$16</c:f>
+              <c:f>Figures!$H$3:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1085,7 +1394,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
+              <c:f>Figures!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1165,7 +1474,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$3:$B$16</c:f>
+              <c:f>Figures!$A$3:$B$16</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
@@ -1231,7 +1540,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$16</c:f>
+              <c:f>Figures!$I$3:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1288,7 +1597,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="59"/>
         <c:overlap val="-27"/>
         <c:axId val="21650815"/>
         <c:axId val="96254095"/>
@@ -1519,7 +1828,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>BOW + lemmatization</a:t>
+              <a:t>BOW</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> + Rating</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> + Lemmatization</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1565,7 +1882,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$2</c:f>
+              <c:f>Figures!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1643,7 +1960,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$3:$B$16</c:f>
+              <c:f>Figures!$A$3:$B$16</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
@@ -1709,7 +2026,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$16</c:f>
+              <c:f>Figures!$M$3:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1763,7 +2080,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$2</c:f>
+              <c:f>Figures!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1843,7 +2160,7 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$3:$B$16</c:f>
+              <c:f>Figures!$A$3:$B$16</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="14"/>
                 <c:lvl>
@@ -1909,7 +2226,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$3:$N$16</c:f>
+              <c:f>Figures!$N$3:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1966,7 +2283,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="59"/>
         <c:overlap val="-27"/>
         <c:axId val="21650815"/>
         <c:axId val="96254095"/>
@@ -4207,8 +4524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D211AB2F-F0AE-45B6-A6F5-0A0103D1A4A9}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M8" workbookViewId="0">
-      <selection activeCell="AD41" sqref="AD41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4654,4 +4971,500 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4F5B0-99D3-420C-BF49-84BE54B6AEF0}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.71</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0.41</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.69</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.41</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.62</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.49</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.71</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.77</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="9">
+        <v>36</v>
+      </c>
+      <c r="J7" s="34">
+        <f>I7/SUM($I$7:$I$10)</f>
+        <v>8.0178173719376397E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.13</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.21</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="9">
+        <v>56</v>
+      </c>
+      <c r="J8" s="34">
+        <f>I8/SUM($I$7:$I$10)</f>
+        <v>0.12472160356347439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.43</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.49</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="9">
+        <v>115</v>
+      </c>
+      <c r="J9" s="34">
+        <f>I9/SUM($I$7:$I$10)</f>
+        <v>0.25612472160356348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.78</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="39">
+        <v>242</v>
+      </c>
+      <c r="J10" s="35">
+        <f>I10/SUM($I$7:$I$10)</f>
+        <v>0.53897550111358572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.13</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.49</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.73</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0.76</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>